<commit_message>
Updated thickness function, figures, etc. for paper
</commit_message>
<xml_diff>
--- a/EPSILONREGRESSION_FINAL/EpsilonRegression.xlsx
+++ b/EPSILONREGRESSION_FINAL/EpsilonRegression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahcshi/Documents/GitHub/BASELINES/EPSILONREGRESSION_FINAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90007B39-6E2C-FB4E-9E02-DCA5492C3FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDB4487-84EE-324F-9570-62935FAB4450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22860" windowHeight="20700" activeTab="3" xr2:uid="{FEE6C955-F107-534A-8F98-4BC8B7F4190E}"/>
+    <workbookView xWindow="36900" yWindow="500" windowWidth="44660" windowHeight="28300" activeTab="3" xr2:uid="{FEE6C955-F107-534A-8F98-4BC8B7F4190E}"/>
   </bookViews>
   <sheets>
     <sheet name="3550Regress" sheetId="2" r:id="rId1"/>
@@ -14633,8 +14633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788A2467-0788-484D-845B-3810F985C6E7}">
   <dimension ref="A1:BS38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>